<commit_message>
added 1 more data column
</commit_message>
<xml_diff>
--- a/data/Sample_Paragraphs.xlsx
+++ b/data/Sample_Paragraphs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t xml:space="preserve">Book Title</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
   </si>
   <si>
     <t xml:space="preserve">Author</t>
@@ -45,6 +48,9 @@
     <t xml:space="preserve">Mr. Springer</t>
   </si>
   <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
     <t xml:space="preserve">John Updike</t>
   </si>
   <si>
@@ -52,7 +58,7 @@
   </si>
   <si>
     <t xml:space="preserve">“What’s the matter?” I says. “I never knew you to be this anxious about anybody. You must expect some money from Sarah.”
-“She said she —” she says. “Please, Jason,” she shays, “Did I?”
+“She said she —” Emily says. “Please, Jason,” she shays, “Did I?”
 “You must have been to school today, after all,” I says, “Somewhere where they taught you to say please. Wait a minute, while I wait on that customer.”
 I went and waited on him. When I turned to come back she was out of sight behind the desk. I ran. I ran around the  desk and caught her as she jered her hand out of the drawer. I took the letter away from her, beating her knuckles on the desk until she let go.
 “You would, would you?” I says.
@@ -63,7 +69,10 @@
 “She said she would,” she says, “Give it to me. Please, Jason. I won't ever ask you anything again, if you’ll give it to me this time.”</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarah</t>
+    <t xml:space="preserve">Emily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
   </si>
   <si>
     <t xml:space="preserve">William Faulkner</t>
@@ -341,22 +350,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -369,131 +378,161 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="507.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="235.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="458" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="297.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="778.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="458" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="272.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="495.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>38</v>
+      <c r="E10" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>